<commit_message>
GP03FLMA changed cal sheet to remove m from depth
</commit_message>
<xml_diff>
--- a/GP03FLMA/Omaha_Cal_Info_GP03FLMA_00001.xlsx
+++ b/GP03FLMA/Omaha_Cal_Info_GP03FLMA_00001.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Repaired GIT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18816" windowHeight="8040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="81">
   <si>
     <t>Ref Des</t>
   </si>
@@ -60,9 +54,6 @@
   </si>
   <si>
     <t>GP03FLMA-00001</t>
-  </si>
-  <si>
-    <t>4127m</t>
   </si>
   <si>
     <t>Melville 130</t>
@@ -203,12 +194,6 @@
     <t>10262</t>
   </si>
   <si>
-    <t>49.9795 N</t>
-  </si>
-  <si>
-    <t>144.254 W</t>
-  </si>
-  <si>
     <t>GP03FLMA-RIS01-05-FLORTD000</t>
   </si>
   <si>
@@ -268,16 +253,22 @@
   <si>
     <t>This serial number is made up until we can find the real serial number</t>
   </si>
+  <si>
+    <t>49° 58.76' N</t>
+  </si>
+  <si>
+    <t>144° 15.25' W</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="d\-mmm\-yy;@"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -331,6 +322,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -435,12 +438,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -468,7 +472,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -483,7 +487,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="19" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -504,10 +508,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -594,9 +598,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 15" xfId="3"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
@@ -936,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -946,29 +955,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="9"/>
-    <col min="2" max="2" width="15.6640625" style="9"/>
-    <col min="3" max="3" width="15.6640625" style="10"/>
-    <col min="4" max="4" width="11.33203125" style="11"/>
-    <col min="5" max="5" width="11.33203125" style="12"/>
+    <col min="1" max="1" width="22.28515625" style="9"/>
+    <col min="2" max="2" width="15.7109375" style="9"/>
+    <col min="3" max="3" width="15.7109375" style="10"/>
+    <col min="4" max="4" width="11.28515625" style="11"/>
+    <col min="5" max="5" width="11.28515625" style="12"/>
     <col min="6" max="6" width="11" style="11"/>
-    <col min="7" max="7" width="11.88671875" style="9"/>
-    <col min="8" max="8" width="13.5546875" style="9"/>
-    <col min="9" max="9" width="12.6640625" style="9"/>
-    <col min="10" max="10" width="11.5546875" style="9"/>
-    <col min="11" max="11" width="18.5546875" style="9"/>
-    <col min="12" max="12" width="13.44140625" style="9"/>
-    <col min="13" max="13" width="12.5546875" style="9"/>
-    <col min="14" max="1025" width="8.88671875" style="9"/>
+    <col min="7" max="7" width="11.85546875" style="9"/>
+    <col min="8" max="8" width="13.5703125" style="9"/>
+    <col min="9" max="9" width="12.7109375" style="9"/>
+    <col min="10" max="10" width="11.5703125" style="9"/>
+    <col min="11" max="11" width="18.5703125" style="9"/>
+    <col min="12" max="12" width="13.42578125" style="9"/>
+    <col min="13" max="13" width="12.5703125" style="9"/>
+    <col min="14" max="1025" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1016,7 @@
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
     </row>
-    <row r="2" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1026,20 +1035,20 @@
       <c r="F2" s="23">
         <v>41807</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>60</v>
+      <c r="G2" s="54" t="s">
+        <v>79</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>61</v>
+      <c r="H2" s="54" t="s">
+        <v>80</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="22">
+        <v>4127</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="25" t="s">
         <v>14</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>15</v>
       </c>
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
@@ -1056,42 +1065,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F11"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="29"/>
-    <col min="2" max="2" width="21.44140625" style="29"/>
-    <col min="3" max="3" width="19.109375" style="30"/>
-    <col min="4" max="4" width="20.109375" style="29"/>
-    <col min="5" max="5" width="29.109375" style="29"/>
+    <col min="1" max="1" width="28.85546875" style="29"/>
+    <col min="2" max="2" width="21.42578125" style="29"/>
+    <col min="3" max="3" width="19.140625" style="30"/>
+    <col min="4" max="4" width="20.140625" style="29"/>
+    <col min="5" max="5" width="29.140625" style="29"/>
     <col min="6" max="6" width="31" style="29"/>
-    <col min="7" max="7" width="10.6640625" style="30"/>
-    <col min="8" max="11" width="10.6640625" style="29"/>
+    <col min="7" max="7" width="10.7109375" style="30"/>
+    <col min="8" max="11" width="10.7109375" style="29"/>
     <col min="12" max="12" width="5" style="29"/>
-    <col min="13" max="1025" width="8.88671875" style="29"/>
+    <col min="13" max="1025" width="8.85546875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="36" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1024" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>19</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>10</v>
@@ -1103,7 +1112,7 @@
       <c r="L1" s="35"/>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="38"/>
@@ -2129,9 +2138,9 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>12</v>
@@ -2143,13 +2152,13 @@
         <v>1005</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="39">
         <v>2.1179999999999999E-6</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="29">
         <v>29</v>
@@ -3171,9 +3180,9 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>12</v>
@@ -3185,13 +3194,13 @@
         <v>1005</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="39">
         <v>54</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -4211,9 +4220,9 @@
       <c r="AMI4"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5" s="41" t="s">
         <v>12</v>
@@ -4225,7 +4234,7 @@
         <v>1005</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="42">
         <v>1.21E-2</v>
@@ -5249,9 +5258,9 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B6" s="41" t="s">
         <v>12</v>
@@ -5263,7 +5272,7 @@
         <v>1005</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="42">
         <v>53</v>
@@ -6287,9 +6296,9 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="41" t="s">
         <v>12</v>
@@ -6301,7 +6310,7 @@
         <v>1005</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="42">
         <v>9.11E-2</v>
@@ -7325,9 +7334,9 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="41" t="s">
         <v>12</v>
@@ -7339,7 +7348,7 @@
         <v>1005</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="43">
         <v>50</v>
@@ -8363,9 +8372,9 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9" s="41" t="s">
         <v>12</v>
@@ -8377,13 +8386,13 @@
         <v>1005</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7">
         <v>124</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -9403,9 +9412,9 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>12</v>
@@ -9417,13 +9426,13 @@
         <v>1005</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="43">
         <v>700</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -10443,9 +10452,9 @@
       <c r="AMI10"/>
       <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>12</v>
@@ -10457,13 +10466,13 @@
         <v>1005</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7">
         <v>1.0760000000000001</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -11483,9 +11492,9 @@
       <c r="AMI11"/>
       <c r="AMJ11"/>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="41" t="s">
         <v>12</v>
@@ -11497,13 +11506,13 @@
         <v>1005</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="43">
         <v>3.9E-2</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -12523,9 +12532,9 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>63</v>
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>60</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>12</v>
@@ -12537,13 +12546,13 @@
         <v>80</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="39">
         <v>17533</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="29">
         <v>29</v>
@@ -13565,11 +13574,11 @@
       <c r="AMI13"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
-        <v>63</v>
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>60</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="30">
@@ -13579,7 +13588,7 @@
         <v>80</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="39">
         <v>2229</v>
@@ -14603,11 +14612,11 @@
       <c r="AMI14"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>63</v>
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>60</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="30">
@@ -14617,7 +14626,7 @@
         <v>80</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="42">
         <v>101</v>
@@ -15641,11 +15650,11 @@
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
-        <v>63</v>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>60</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="30">
@@ -15655,7 +15664,7 @@
         <v>80</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="42">
         <v>38502</v>
@@ -16679,11 +16688,11 @@
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
-        <v>63</v>
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>60</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="30">
@@ -16693,7 +16702,7 @@
         <v>80</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="42">
         <v>1</v>
@@ -17717,11 +17726,11 @@
       <c r="AMI17"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A18" s="41" t="s">
-        <v>63</v>
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>60</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="30">
@@ -17731,7 +17740,7 @@
         <v>80</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="43">
         <v>0</v>
@@ -18755,11 +18764,11 @@
       <c r="AMI18"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
-        <v>63</v>
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>60</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="30">
@@ -18769,13 +18778,13 @@
         <v>80</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="43">
         <v>35</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -19795,9 +19804,9 @@
       <c r="AMI19"/>
       <c r="AMJ19"/>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>12</v>
@@ -19809,13 +19818,13 @@
         <v>129</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="39">
         <v>49.97945</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="29">
         <v>29</v>
@@ -20837,9 +20846,9 @@
       <c r="AMI20"/>
       <c r="AMJ20"/>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="41" t="s">
         <v>12</v>
@@ -20851,13 +20860,13 @@
         <v>129</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21" s="39">
         <v>-144.254166666667</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -21877,9 +21886,9 @@
       <c r="AMI21"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="41" t="s">
         <v>12</v>
@@ -21891,10 +21900,10 @@
         <v>129</v>
       </c>
       <c r="E22" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
@@ -22915,7 +22924,7 @@
       <c r="AMI22"/>
       <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="41"/>
       <c r="C23" s="22"/>
@@ -23941,9 +23950,9 @@
       <c r="AMI23"/>
       <c r="AMJ23"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>12</v>
@@ -23955,13 +23964,13 @@
         <v>18351</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="39">
         <v>49.97945</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="29">
         <v>500</v>
@@ -24983,9 +24992,9 @@
       <c r="AMI24"/>
       <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>12</v>
@@ -24997,7 +25006,7 @@
         <v>18351</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="39">
         <v>-144.254166666667</v>
@@ -26021,9 +26030,9 @@
       <c r="AMI25"/>
       <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>12</v>
@@ -26035,7 +26044,7 @@
         <v>18351</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="39">
         <v>49.97945</v>
@@ -27059,9 +27068,9 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>12</v>
@@ -27073,7 +27082,7 @@
         <v>18351</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="39">
         <v>-144.254166666667</v>
@@ -28097,9 +28106,9 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>12</v>
@@ -28111,7 +28120,7 @@
         <v>18351</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" s="42">
         <v>5000</v>
@@ -29135,9 +29144,9 @@
       <c r="AMI28"/>
       <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B29" s="41" t="s">
         <v>12</v>
@@ -29149,7 +29158,7 @@
         <v>18351</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="42">
         <v>0.45</v>
@@ -30173,9 +30182,9 @@
       <c r="AMI29"/>
       <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B30" s="41" t="s">
         <v>12</v>
@@ -30187,7 +30196,7 @@
         <v>18351</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="42">
         <v>0.45</v>
@@ -31211,9 +31220,9 @@
       <c r="AMI30"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>12</v>
@@ -31225,7 +31234,7 @@
         <v>18351</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" s="42">
         <v>0.45</v>
@@ -32249,9 +32258,9 @@
       <c r="AMI31"/>
       <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" s="41" t="s">
         <v>12</v>
@@ -32263,7 +32272,7 @@
         <v>18351</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="42">
         <v>0.45</v>
@@ -33287,9 +33296,9 @@
       <c r="AMI32"/>
       <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>12</v>
@@ -33298,16 +33307,16 @@
         <v>1</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="2">
         <v>1450</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H33" s="29">
         <v>29</v>
@@ -34329,9 +34338,9 @@
       <c r="AMI33"/>
       <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="41" t="s">
         <v>12</v>
@@ -34340,10 +34349,10 @@
         <v>1</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" s="39">
         <v>49.97945</v>
@@ -35367,9 +35376,9 @@
       <c r="AMI34"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35" s="41" t="s">
         <v>12</v>
@@ -35378,10 +35387,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F35" s="39">
         <v>-144.254166666667</v>
@@ -36405,9 +36414,9 @@
       <c r="AMI35"/>
       <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B36" s="41" t="s">
         <v>12</v>
@@ -36416,10 +36425,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F36" s="39">
         <v>57</v>
@@ -37443,9 +37452,9 @@
       <c r="AMI36"/>
       <c r="AMJ36"/>
     </row>
-    <row r="37" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>12</v>
@@ -37457,13 +37466,13 @@
         <v>10220</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37" s="2">
         <v>1450</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H37" s="22">
         <v>39</v>
@@ -38485,9 +38494,9 @@
       <c r="AMI37"/>
       <c r="AMJ37"/>
     </row>
-    <row r="38" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>12</v>
@@ -38499,7 +38508,7 @@
         <v>10220</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" s="39">
         <v>49.97945</v>
@@ -39523,9 +39532,9 @@
       <c r="AMI38"/>
       <c r="AMJ38"/>
     </row>
-    <row r="39" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>12</v>
@@ -39537,7 +39546,7 @@
         <v>10220</v>
       </c>
       <c r="E39" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39" s="39">
         <v>-144.254166666667</v>
@@ -40561,9 +40570,9 @@
       <c r="AMI39"/>
       <c r="AMJ39"/>
     </row>
-    <row r="40" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>12</v>
@@ -40575,7 +40584,7 @@
         <v>10220</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F40" s="39">
         <v>20</v>
@@ -41599,9 +41608,9 @@
       <c r="AMI40"/>
       <c r="AMJ40"/>
     </row>
-    <row r="41" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>12</v>
@@ -41613,13 +41622,13 @@
         <v>10260</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F41" s="2">
         <v>1450</v>
       </c>
       <c r="G41" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H41" s="22">
         <v>59</v>
@@ -42641,9 +42650,9 @@
       <c r="AMI41"/>
       <c r="AMJ41"/>
     </row>
-    <row r="42" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>12</v>
@@ -42655,7 +42664,7 @@
         <v>10260</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42" s="39">
         <v>49.97945</v>
@@ -43679,9 +43688,9 @@
       <c r="AMI42"/>
       <c r="AMJ42"/>
     </row>
-    <row r="43" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B43" s="41" t="s">
         <v>12</v>
@@ -43693,7 +43702,7 @@
         <v>10260</v>
       </c>
       <c r="E43" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F43" s="39">
         <v>-144.254166666667</v>
@@ -44717,9 +44726,9 @@
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>12</v>
@@ -44731,7 +44740,7 @@
         <v>10260</v>
       </c>
       <c r="E44" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F44" s="39">
         <v>60</v>
@@ -45755,9 +45764,9 @@
       <c r="AMI44"/>
       <c r="AMJ44"/>
     </row>
-    <row r="45" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>12</v>
@@ -45769,13 +45778,13 @@
         <v>10215</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F45" s="2">
         <v>1450</v>
       </c>
       <c r="G45" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H45" s="22">
         <v>90</v>
@@ -46797,9 +46806,9 @@
       <c r="AMI45"/>
       <c r="AMJ45"/>
     </row>
-    <row r="46" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>12</v>
@@ -46811,7 +46820,7 @@
         <v>10215</v>
       </c>
       <c r="E46" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F46" s="39">
         <v>49.97945</v>
@@ -47835,9 +47844,9 @@
       <c r="AMI46"/>
       <c r="AMJ46"/>
     </row>
-    <row r="47" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>12</v>
@@ -47849,7 +47858,7 @@
         <v>10215</v>
       </c>
       <c r="E47" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F47" s="39">
         <v>-144.254166666667</v>
@@ -48873,9 +48882,9 @@
       <c r="AMI47"/>
       <c r="AMJ47"/>
     </row>
-    <row r="48" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>12</v>
@@ -48887,7 +48896,7 @@
         <v>10215</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F48" s="39">
         <v>15</v>
@@ -49911,9 +49920,9 @@
       <c r="AMI48"/>
       <c r="AMJ48"/>
     </row>
-    <row r="49" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>12</v>
@@ -49922,16 +49931,16 @@
         <v>1</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F49" s="2">
         <v>1450</v>
       </c>
       <c r="G49" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H49" s="22">
         <v>130</v>
@@ -50953,9 +50962,9 @@
       <c r="AMI49"/>
       <c r="AMJ49"/>
     </row>
-    <row r="50" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>12</v>
@@ -50964,10 +50973,10 @@
         <v>1</v>
       </c>
       <c r="D50" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="39">
         <v>49.97945</v>
@@ -51991,9 +52000,9 @@
       <c r="AMI50"/>
       <c r="AMJ50"/>
     </row>
-    <row r="51" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>12</v>
@@ -52002,10 +52011,10 @@
         <v>1</v>
       </c>
       <c r="D51" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F51" s="39">
         <v>-144.254166666667</v>
@@ -53029,9 +53038,9 @@
       <c r="AMI51"/>
       <c r="AMJ51"/>
     </row>
-    <row r="52" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A52" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B52" s="41" t="s">
         <v>12</v>
@@ -53040,10 +53049,10 @@
         <v>1</v>
       </c>
       <c r="D52" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F52" s="39">
         <v>54</v>
@@ -54067,9 +54076,9 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>12</v>
@@ -54078,16 +54087,16 @@
         <v>1</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F53" s="2">
         <v>1450</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H53" s="22">
         <v>180</v>
@@ -55109,9 +55118,9 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A54" s="41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B54" s="41" t="s">
         <v>12</v>
@@ -55120,10 +55129,10 @@
         <v>1</v>
       </c>
       <c r="D54" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F54" s="39">
         <v>49.97945</v>
@@ -56147,9 +56156,9 @@
       <c r="AMI54"/>
       <c r="AMJ54"/>
     </row>
-    <row r="55" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A55" s="41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B55" s="41" t="s">
         <v>12</v>
@@ -56158,10 +56167,10 @@
         <v>1</v>
       </c>
       <c r="D55" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E55" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F55" s="39">
         <v>-144.254166666667</v>
@@ -57185,9 +57194,9 @@
       <c r="AMI55"/>
       <c r="AMJ55"/>
     </row>
-    <row r="56" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A56" s="41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B56" s="41" t="s">
         <v>12</v>
@@ -57196,10 +57205,10 @@
         <v>1</v>
       </c>
       <c r="D56" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E56" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F56" s="39">
         <v>62</v>
@@ -58223,9 +58232,9 @@
       <c r="AMI56"/>
       <c r="AMJ56"/>
     </row>
-    <row r="57" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B57" s="22" t="s">
         <v>12</v>
@@ -58237,13 +58246,13 @@
         <v>10252</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F57" s="2">
         <v>1450</v>
       </c>
       <c r="G57" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H57" s="22">
         <v>250</v>
@@ -59265,9 +59274,9 @@
       <c r="AMI57"/>
       <c r="AMJ57"/>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A58" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B58" s="41" t="s">
         <v>12</v>
@@ -59279,7 +59288,7 @@
         <v>10252</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F58" s="39">
         <v>49.97945</v>
@@ -60303,9 +60312,9 @@
       <c r="AMI58"/>
       <c r="AMJ58"/>
     </row>
-    <row r="59" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A59" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B59" s="41" t="s">
         <v>12</v>
@@ -60317,7 +60326,7 @@
         <v>10252</v>
       </c>
       <c r="E59" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F59" s="39">
         <v>-144.254166666667</v>
@@ -61341,9 +61350,9 @@
       <c r="AMI59"/>
       <c r="AMJ59"/>
     </row>
-    <row r="60" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A60" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>12</v>
@@ -61355,7 +61364,7 @@
         <v>10252</v>
       </c>
       <c r="E60" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F60" s="39">
         <v>52</v>
@@ -62379,9 +62388,9 @@
       <c r="AMI60"/>
       <c r="AMJ60"/>
     </row>
-    <row r="61" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>12</v>
@@ -62393,13 +62402,13 @@
         <v>10219</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F61" s="2">
         <v>1450</v>
       </c>
       <c r="G61" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H61" s="22">
         <v>350</v>
@@ -63421,9 +63430,9 @@
       <c r="AMI61"/>
       <c r="AMJ61"/>
     </row>
-    <row r="62" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A62" s="41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B62" s="41" t="s">
         <v>12</v>
@@ -63435,7 +63444,7 @@
         <v>10219</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F62" s="39">
         <v>49.97945</v>
@@ -64459,9 +64468,9 @@
       <c r="AMI62"/>
       <c r="AMJ62"/>
     </row>
-    <row r="63" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A63" s="41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B63" s="41" t="s">
         <v>12</v>
@@ -64473,7 +64482,7 @@
         <v>10219</v>
       </c>
       <c r="E63" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F63" s="39">
         <v>-144.254166666667</v>
@@ -65497,9 +65506,9 @@
       <c r="AMI63"/>
       <c r="AMJ63"/>
     </row>
-    <row r="64" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A64" s="41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B64" s="41" t="s">
         <v>12</v>
@@ -65511,7 +65520,7 @@
         <v>10219</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F64" s="39">
         <v>19</v>
@@ -66535,9 +66544,9 @@
       <c r="AMI64"/>
       <c r="AMJ64"/>
     </row>
-    <row r="65" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>12</v>
@@ -66549,13 +66558,13 @@
         <v>10256</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F65" s="2">
         <v>1450</v>
       </c>
       <c r="G65" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H65" s="22">
         <v>501</v>
@@ -67577,9 +67586,9 @@
       <c r="AMI65"/>
       <c r="AMJ65"/>
     </row>
-    <row r="66" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B66" s="41" t="s">
         <v>12</v>
@@ -67591,7 +67600,7 @@
         <v>10256</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F66" s="39">
         <v>49.97945</v>
@@ -68615,9 +68624,9 @@
       <c r="AMI66"/>
       <c r="AMJ66"/>
     </row>
-    <row r="67" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A67" s="41" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B67" s="41" t="s">
         <v>12</v>
@@ -68629,7 +68638,7 @@
         <v>10256</v>
       </c>
       <c r="E67" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F67" s="39">
         <v>-144.254166666667</v>
@@ -69653,9 +69662,9 @@
       <c r="AMI67"/>
       <c r="AMJ67"/>
     </row>
-    <row r="68" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A68" s="41" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B68" s="41" t="s">
         <v>12</v>
@@ -69667,7 +69676,7 @@
         <v>10256</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F68" s="39">
         <v>56</v>
@@ -70691,9 +70700,9 @@
       <c r="AMI68"/>
       <c r="AMJ68"/>
     </row>
-    <row r="69" spans="1:1024" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1024" s="51" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>12</v>
@@ -70705,22 +70714,22 @@
         <v>10226</v>
       </c>
       <c r="E69" s="49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F69" s="1">
         <v>5076</v>
       </c>
       <c r="G69" s="50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H69" s="48">
         <v>748</v>
       </c>
       <c r="J69" s="48"/>
     </row>
-    <row r="70" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A70" s="41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B70" s="52" t="s">
         <v>12</v>
@@ -70732,7 +70741,7 @@
         <v>10226</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F70" s="39">
         <v>49.97945</v>
@@ -70741,9 +70750,9 @@
       <c r="H70"/>
       <c r="J70" s="22"/>
     </row>
-    <row r="71" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A71" s="41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B71" s="52" t="s">
         <v>12</v>
@@ -70755,7 +70764,7 @@
         <v>10226</v>
       </c>
       <c r="E71" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F71" s="39">
         <v>-144.254166666667</v>
@@ -70764,9 +70773,9 @@
       <c r="H71"/>
       <c r="J71" s="22"/>
     </row>
-    <row r="72" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B72" s="52" t="s">
         <v>12</v>
@@ -70778,7 +70787,7 @@
         <v>10226</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F72" s="39">
         <v>26</v>
@@ -70787,9 +70796,9 @@
       <c r="H72"/>
       <c r="J72" s="22"/>
     </row>
-    <row r="73" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>12</v>
@@ -70801,22 +70810,22 @@
         <v>10229</v>
       </c>
       <c r="E73" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F73" s="1">
         <v>5076</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H73" s="22">
         <v>999</v>
       </c>
       <c r="J73" s="22"/>
     </row>
-    <row r="74" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A74" s="41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B74" s="41" t="s">
         <v>12</v>
@@ -70828,7 +70837,7 @@
         <v>10229</v>
       </c>
       <c r="E74" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F74" s="39">
         <v>49.97945</v>
@@ -70837,9 +70846,9 @@
       <c r="H74"/>
       <c r="J74" s="22"/>
     </row>
-    <row r="75" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B75" s="41" t="s">
         <v>12</v>
@@ -70851,7 +70860,7 @@
         <v>10229</v>
       </c>
       <c r="E75" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F75" s="39">
         <v>-144.254166666667</v>
@@ -70860,9 +70869,9 @@
       <c r="H75"/>
       <c r="J75" s="22"/>
     </row>
-    <row r="76" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A76" s="41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B76" s="41" t="s">
         <v>12</v>
@@ -70874,7 +70883,7 @@
         <v>10229</v>
       </c>
       <c r="E76" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F76" s="39">
         <v>29</v>
@@ -70883,9 +70892,9 @@
       <c r="H76"/>
       <c r="J76" s="22"/>
     </row>
-    <row r="77" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>12</v>
@@ -70897,22 +70906,22 @@
         <v>10267</v>
       </c>
       <c r="E77" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F77" s="1">
         <v>5076</v>
       </c>
       <c r="G77" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H77" s="22">
         <v>1501</v>
       </c>
       <c r="J77" s="22"/>
     </row>
-    <row r="78" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B78" s="41" t="s">
         <v>12</v>
@@ -70924,16 +70933,16 @@
         <v>10267</v>
       </c>
       <c r="E78" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F78" s="39">
         <v>49.97945</v>
       </c>
       <c r="J78" s="22"/>
     </row>
-    <row r="79" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B79" s="41" t="s">
         <v>12</v>
@@ -70945,16 +70954,16 @@
         <v>10267</v>
       </c>
       <c r="E79" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F79" s="39">
         <v>-144.254166666667</v>
       </c>
       <c r="J79" s="22"/>
     </row>
-    <row r="80" spans="1:1024" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A80" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B80" s="41" t="s">
         <v>12</v>
@@ -70966,19 +70975,19 @@
         <v>10267</v>
       </c>
       <c r="E80" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F80" s="39">
         <v>67</v>
       </c>
       <c r="J80" s="22"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J81" s="22"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>12</v>
@@ -70987,15 +70996,15 @@
         <v>1</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>12</v>
@@ -71004,10 +71013,10 @@
         <v>1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redmine #9194 Cal sheets for GP03FLMA deployments 1-3 changed/added to repo.
</commit_message>
<xml_diff>
--- a/GP03FLMA/Omaha_Cal_Info_GP03FLMA_00001.xlsx
+++ b/GP03FLMA/Omaha_Cal_Info_GP03FLMA_00001.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8040"/>
+    <workbookView xWindow="10720" yWindow="7720" windowWidth="24960" windowHeight="12620"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="82">
   <si>
     <t>Ref Des</t>
   </si>
@@ -54,9 +59,6 @@
   </si>
   <si>
     <t>GP03FLMA-00001</t>
-  </si>
-  <si>
-    <t>Melville 130</t>
   </si>
   <si>
     <t>Mooring Serial Number</t>
@@ -236,12 +238,6 @@
     <t>GP03FLMA-RIM01-02-CTDMOH067</t>
   </si>
   <si>
-    <t>GP03FLMA-FMM01-01-SIOENG000</t>
-  </si>
-  <si>
-    <t>GP03FLMA-FMS01-01-SIOENG000</t>
-  </si>
-  <si>
     <t>GP03FLMA-00001-FMM01</t>
   </si>
   <si>
@@ -251,13 +247,65 @@
     <t>This serial number is made up until we can find the real serial number</t>
   </si>
   <si>
-    <t>49° 58.76' N</t>
+    <t xml:space="preserve">There was no data received from GP03FLMA during D00001.  It was speculated to be a batery issue on the mooring. </t>
   </si>
   <si>
-    <t>144° 15.25' W</t>
+    <t>144° 15.24' W</t>
   </si>
   <si>
-    <t xml:space="preserve">There was no data received from GP03FLMA during D00001.  It was speculated to be a batery issue on the mooring. </t>
+    <t>49° 58.77' N</t>
+  </si>
+  <si>
+    <t>MV-130</t>
+  </si>
+  <si>
+    <t>Units in mm</t>
+  </si>
+  <si>
+    <r>
+      <t>GP03FLMA-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>M01-01-SIOENG000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>GP03FLMA-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>RI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>S01-01-SIOENG000</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -268,7 +316,7 @@
     <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -331,9 +379,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -438,13 +496,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -602,10 +661,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 15" xfId="3"/>
+    <cellStyle name="Normal 2 5 2" xfId="4"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
@@ -733,7 +805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -768,7 +840,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -955,29 +1027,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="9"/>
-    <col min="2" max="2" width="15.7109375" style="9"/>
-    <col min="3" max="3" width="15.7109375" style="10"/>
-    <col min="4" max="4" width="11.28515625" style="11"/>
-    <col min="5" max="5" width="11.28515625" style="12"/>
-    <col min="6" max="6" width="11" style="11"/>
-    <col min="7" max="7" width="11.85546875" style="9"/>
-    <col min="8" max="8" width="13.5703125" style="9"/>
-    <col min="9" max="9" width="12.7109375" style="9"/>
-    <col min="10" max="10" width="11.5703125" style="9"/>
-    <col min="11" max="11" width="18.5703125" style="9"/>
-    <col min="12" max="12" width="13.42578125" style="9"/>
-    <col min="13" max="13" width="12.5703125" style="9"/>
-    <col min="14" max="1025" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="11.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="11" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="9" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" style="9"/>
+    <col min="11" max="11" width="44.1640625" style="9" customWidth="1"/>
+    <col min="12" max="1025" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="20" customFormat="1" ht="28">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1084,7 @@
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
     </row>
-    <row r="2" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="28" customFormat="1">
       <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1032,23 +1100,23 @@
       <c r="E2" s="24">
         <v>0.94722222222222197</v>
       </c>
-      <c r="F2" s="23">
-        <v>41807</v>
+      <c r="F2" s="56">
+        <v>41805</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I2" s="22">
         <v>4127</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>13</v>
+      <c r="J2" s="55" t="s">
+        <v>78</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
@@ -1058,6 +1126,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1065,42 +1138,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK83"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="29"/>
-    <col min="2" max="2" width="21.42578125" style="29"/>
-    <col min="3" max="3" width="19.140625" style="30"/>
-    <col min="4" max="4" width="20.140625" style="29"/>
-    <col min="5" max="5" width="29.140625" style="29"/>
-    <col min="6" max="6" width="31" style="29"/>
-    <col min="7" max="7" width="10.7109375" style="30"/>
-    <col min="8" max="11" width="10.7109375" style="29"/>
-    <col min="12" max="12" width="5" style="29"/>
-    <col min="13" max="1025" width="8.85546875" style="29"/>
+    <col min="1" max="1" width="29" style="29" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="11" style="30" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="31.5" style="29" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="29" customWidth="1"/>
+    <col min="7" max="7" width="17" style="30" customWidth="1"/>
+    <col min="8" max="1025" width="8.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="36" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" s="36" customFormat="1" ht="28">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>17</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>10</v>
@@ -1112,7 +1186,7 @@
       <c r="L1" s="35"/>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="38"/>
@@ -2138,9 +2212,9 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024">
       <c r="A3" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>12</v>
@@ -2152,13 +2226,13 @@
         <v>1005</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="39">
         <v>2.1179999999999999E-6</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="29">
         <v>29</v>
@@ -3180,9 +3254,9 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024">
       <c r="A4" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>12</v>
@@ -3194,13 +3268,13 @@
         <v>1005</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="39">
         <v>54</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -4220,9 +4294,9 @@
       <c r="AMI4"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024">
       <c r="A5" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="41" t="s">
         <v>12</v>
@@ -4234,7 +4308,7 @@
         <v>1005</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="42">
         <v>1.21E-2</v>
@@ -5258,9 +5332,9 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024">
       <c r="A6" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="41" t="s">
         <v>12</v>
@@ -5272,7 +5346,7 @@
         <v>1005</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="42">
         <v>53</v>
@@ -6296,9 +6370,9 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024">
       <c r="A7" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="41" t="s">
         <v>12</v>
@@ -6310,7 +6384,7 @@
         <v>1005</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="42">
         <v>9.11E-2</v>
@@ -7334,9 +7408,9 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1024">
       <c r="A8" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="41" t="s">
         <v>12</v>
@@ -7348,7 +7422,7 @@
         <v>1005</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="43">
         <v>50</v>
@@ -8372,9 +8446,9 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024">
       <c r="A9" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="41" t="s">
         <v>12</v>
@@ -8386,13 +8460,13 @@
         <v>1005</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7">
         <v>124</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -9412,9 +9486,9 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1024">
       <c r="A10" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>12</v>
@@ -9426,13 +9500,13 @@
         <v>1005</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="43">
         <v>700</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -10452,9 +10526,9 @@
       <c r="AMI10"/>
       <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1024">
       <c r="A11" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>12</v>
@@ -10466,13 +10540,13 @@
         <v>1005</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7">
         <v>1.0760000000000001</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -11492,9 +11566,9 @@
       <c r="AMI11"/>
       <c r="AMJ11"/>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1024">
       <c r="A12" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="41" t="s">
         <v>12</v>
@@ -11506,13 +11580,13 @@
         <v>1005</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="43">
         <v>3.9E-2</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -12532,9 +12606,9 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1024">
       <c r="A13" s="53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>12</v>
@@ -12546,13 +12620,13 @@
         <v>80</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="39">
         <v>17533</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="29">
         <v>29</v>
@@ -13574,9 +13648,9 @@
       <c r="AMI13"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1024">
       <c r="A14" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>12</v>
@@ -13588,7 +13662,7 @@
         <v>80</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="39">
         <v>2229</v>
@@ -14612,9 +14686,9 @@
       <c r="AMI14"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1024">
       <c r="A15" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>12</v>
@@ -14626,7 +14700,7 @@
         <v>80</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="42">
         <v>101</v>
@@ -15650,9 +15724,9 @@
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1024">
       <c r="A16" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>12</v>
@@ -15664,7 +15738,7 @@
         <v>80</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="42">
         <v>38502</v>
@@ -16688,9 +16762,9 @@
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1024">
       <c r="A17" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>12</v>
@@ -16702,7 +16776,7 @@
         <v>80</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="42">
         <v>1</v>
@@ -17726,9 +17800,9 @@
       <c r="AMI17"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1024">
       <c r="A18" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>12</v>
@@ -17740,7 +17814,7 @@
         <v>80</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="43">
         <v>0</v>
@@ -18764,9 +18838,9 @@
       <c r="AMI18"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1024">
       <c r="A19" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>12</v>
@@ -18778,13 +18852,13 @@
         <v>80</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="43">
         <v>35</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -19804,9 +19878,9 @@
       <c r="AMI19"/>
       <c r="AMJ19"/>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1024">
       <c r="A20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>12</v>
@@ -19818,13 +19892,13 @@
         <v>129</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="39">
         <v>49.97945</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="29">
         <v>29</v>
@@ -20846,9 +20920,9 @@
       <c r="AMI20"/>
       <c r="AMJ20"/>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1024">
       <c r="A21" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="41" t="s">
         <v>12</v>
@@ -20860,13 +20934,13 @@
         <v>129</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="39">
         <v>-144.254166666667</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
@@ -21886,9 +21960,9 @@
       <c r="AMI21"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1024">
       <c r="A22" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="41" t="s">
         <v>12</v>
@@ -21900,10 +21974,10 @@
         <v>129</v>
       </c>
       <c r="E22" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
@@ -22924,7 +22998,7 @@
       <c r="AMI22"/>
       <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1024">
       <c r="A23" s="40"/>
       <c r="B23" s="41"/>
       <c r="C23" s="22"/>
@@ -23950,9 +24024,9 @@
       <c r="AMI23"/>
       <c r="AMJ23"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1024">
       <c r="A24" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>12</v>
@@ -23964,13 +24038,13 @@
         <v>18351</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="39">
         <v>49.97945</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="29">
         <v>500</v>
@@ -24992,9 +25066,9 @@
       <c r="AMI24"/>
       <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1024">
       <c r="A25" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>12</v>
@@ -25006,7 +25080,7 @@
         <v>18351</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="39">
         <v>-144.254166666667</v>
@@ -26030,9 +26104,9 @@
       <c r="AMI25"/>
       <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1024">
       <c r="A26" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>12</v>
@@ -26044,7 +26118,7 @@
         <v>18351</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" s="39">
         <v>49.97945</v>
@@ -27068,9 +27142,9 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1024">
       <c r="A27" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>12</v>
@@ -27082,7 +27156,7 @@
         <v>18351</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" s="39">
         <v>-144.254166666667</v>
@@ -28106,9 +28180,9 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1024">
       <c r="A28" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>12</v>
@@ -28120,12 +28194,14 @@
         <v>18351</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
-      <c r="F28" s="42">
-        <v>5000</v>
+      <c r="F28" s="57">
+        <v>500000</v>
       </c>
-      <c r="G28"/>
+      <c r="G28" s="58" t="s">
+        <v>79</v>
+      </c>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28" s="22"/>
@@ -29144,9 +29220,9 @@
       <c r="AMI28"/>
       <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1024">
       <c r="A29" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="41" t="s">
         <v>12</v>
@@ -29158,7 +29234,7 @@
         <v>18351</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="42">
         <v>0.45</v>
@@ -30182,9 +30258,9 @@
       <c r="AMI29"/>
       <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1024">
       <c r="A30" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="41" t="s">
         <v>12</v>
@@ -30196,7 +30272,7 @@
         <v>18351</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" s="42">
         <v>0.45</v>
@@ -31220,9 +31296,9 @@
       <c r="AMI30"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1024">
       <c r="A31" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>12</v>
@@ -31234,7 +31310,7 @@
         <v>18351</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F31" s="42">
         <v>0.45</v>
@@ -32258,9 +32334,9 @@
       <c r="AMI31"/>
       <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1024">
       <c r="A32" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="41" t="s">
         <v>12</v>
@@ -32272,7 +32348,7 @@
         <v>18351</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="42">
         <v>0.45</v>
@@ -33296,9 +33372,9 @@
       <c r="AMI32"/>
       <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1024">
       <c r="A33" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>12</v>
@@ -33307,16 +33383,16 @@
         <v>1</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F33" s="2">
         <v>1450</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H33" s="29">
         <v>29</v>
@@ -34338,9 +34414,9 @@
       <c r="AMI33"/>
       <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1024">
       <c r="A34" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="41" t="s">
         <v>12</v>
@@ -34349,10 +34425,10 @@
         <v>1</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F34" s="39">
         <v>49.97945</v>
@@ -35376,9 +35452,9 @@
       <c r="AMI34"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1024">
       <c r="A35" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="41" t="s">
         <v>12</v>
@@ -35387,10 +35463,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="39">
         <v>-144.254166666667</v>
@@ -36414,9 +36490,9 @@
       <c r="AMI35"/>
       <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1024">
       <c r="A36" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="41" t="s">
         <v>12</v>
@@ -36425,10 +36501,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F36" s="39">
         <v>57</v>
@@ -37452,9 +37528,9 @@
       <c r="AMI36"/>
       <c r="AMJ36"/>
     </row>
-    <row r="37" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1024">
       <c r="A37" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>12</v>
@@ -37466,13 +37542,13 @@
         <v>10220</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F37" s="2">
         <v>1450</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H37" s="22">
         <v>39</v>
@@ -38494,9 +38570,9 @@
       <c r="AMI37"/>
       <c r="AMJ37"/>
     </row>
-    <row r="38" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1024">
       <c r="A38" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>12</v>
@@ -38508,7 +38584,7 @@
         <v>10220</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F38" s="39">
         <v>49.97945</v>
@@ -39532,9 +39608,9 @@
       <c r="AMI38"/>
       <c r="AMJ38"/>
     </row>
-    <row r="39" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1024">
       <c r="A39" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>12</v>
@@ -39546,7 +39622,7 @@
         <v>10220</v>
       </c>
       <c r="E39" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F39" s="39">
         <v>-144.254166666667</v>
@@ -40570,9 +40646,9 @@
       <c r="AMI39"/>
       <c r="AMJ39"/>
     </row>
-    <row r="40" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1024">
       <c r="A40" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>12</v>
@@ -40584,7 +40660,7 @@
         <v>10220</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" s="39">
         <v>20</v>
@@ -41608,9 +41684,9 @@
       <c r="AMI40"/>
       <c r="AMJ40"/>
     </row>
-    <row r="41" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1024">
       <c r="A41" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>12</v>
@@ -41622,13 +41698,13 @@
         <v>10260</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41" s="2">
         <v>1450</v>
       </c>
       <c r="G41" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H41" s="22">
         <v>59</v>
@@ -42650,9 +42726,9 @@
       <c r="AMI41"/>
       <c r="AMJ41"/>
     </row>
-    <row r="42" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1024">
       <c r="A42" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>12</v>
@@ -42664,7 +42740,7 @@
         <v>10260</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F42" s="39">
         <v>49.97945</v>
@@ -43688,9 +43764,9 @@
       <c r="AMI42"/>
       <c r="AMJ42"/>
     </row>
-    <row r="43" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1024">
       <c r="A43" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="41" t="s">
         <v>12</v>
@@ -43702,7 +43778,7 @@
         <v>10260</v>
       </c>
       <c r="E43" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F43" s="39">
         <v>-144.254166666667</v>
@@ -44726,9 +44802,9 @@
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1024">
       <c r="A44" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>12</v>
@@ -44740,7 +44816,7 @@
         <v>10260</v>
       </c>
       <c r="E44" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F44" s="39">
         <v>60</v>
@@ -45764,9 +45840,9 @@
       <c r="AMI44"/>
       <c r="AMJ44"/>
     </row>
-    <row r="45" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1024">
       <c r="A45" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" s="22" t="s">
         <v>12</v>
@@ -45778,13 +45854,13 @@
         <v>10215</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F45" s="2">
         <v>1450</v>
       </c>
       <c r="G45" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H45" s="22">
         <v>90</v>
@@ -46806,9 +46882,9 @@
       <c r="AMI45"/>
       <c r="AMJ45"/>
     </row>
-    <row r="46" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1024">
       <c r="A46" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>12</v>
@@ -46820,7 +46896,7 @@
         <v>10215</v>
       </c>
       <c r="E46" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F46" s="39">
         <v>49.97945</v>
@@ -47844,9 +47920,9 @@
       <c r="AMI46"/>
       <c r="AMJ46"/>
     </row>
-    <row r="47" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1024">
       <c r="A47" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>12</v>
@@ -47858,7 +47934,7 @@
         <v>10215</v>
       </c>
       <c r="E47" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F47" s="39">
         <v>-144.254166666667</v>
@@ -48882,9 +48958,9 @@
       <c r="AMI47"/>
       <c r="AMJ47"/>
     </row>
-    <row r="48" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1024">
       <c r="A48" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>12</v>
@@ -48896,7 +48972,7 @@
         <v>10215</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F48" s="39">
         <v>15</v>
@@ -49920,9 +49996,9 @@
       <c r="AMI48"/>
       <c r="AMJ48"/>
     </row>
-    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1024">
       <c r="A49" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>12</v>
@@ -49931,16 +50007,16 @@
         <v>1</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F49" s="2">
         <v>1450</v>
       </c>
       <c r="G49" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H49" s="22">
         <v>130</v>
@@ -50962,9 +51038,9 @@
       <c r="AMI49"/>
       <c r="AMJ49"/>
     </row>
-    <row r="50" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1024">
       <c r="A50" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>12</v>
@@ -50973,10 +51049,10 @@
         <v>1</v>
       </c>
       <c r="D50" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F50" s="39">
         <v>49.97945</v>
@@ -52000,9 +52076,9 @@
       <c r="AMI50"/>
       <c r="AMJ50"/>
     </row>
-    <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1024">
       <c r="A51" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>12</v>
@@ -52011,10 +52087,10 @@
         <v>1</v>
       </c>
       <c r="D51" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E51" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F51" s="39">
         <v>-144.254166666667</v>
@@ -53038,9 +53114,9 @@
       <c r="AMI51"/>
       <c r="AMJ51"/>
     </row>
-    <row r="52" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1024">
       <c r="A52" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52" s="41" t="s">
         <v>12</v>
@@ -53049,10 +53125,10 @@
         <v>1</v>
       </c>
       <c r="D52" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F52" s="39">
         <v>54</v>
@@ -54076,9 +54152,9 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1024">
       <c r="A53" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>12</v>
@@ -54087,16 +54163,16 @@
         <v>1</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F53" s="2">
         <v>1450</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H53" s="22">
         <v>180</v>
@@ -55118,9 +55194,9 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1024">
       <c r="A54" s="41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" s="41" t="s">
         <v>12</v>
@@ -55129,10 +55205,10 @@
         <v>1</v>
       </c>
       <c r="D54" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F54" s="39">
         <v>49.97945</v>
@@ -56156,9 +56232,9 @@
       <c r="AMI54"/>
       <c r="AMJ54"/>
     </row>
-    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1024">
       <c r="A55" s="41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="41" t="s">
         <v>12</v>
@@ -56167,10 +56243,10 @@
         <v>1</v>
       </c>
       <c r="D55" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F55" s="39">
         <v>-144.254166666667</v>
@@ -57194,9 +57270,9 @@
       <c r="AMI55"/>
       <c r="AMJ55"/>
     </row>
-    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1024">
       <c r="A56" s="41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56" s="41" t="s">
         <v>12</v>
@@ -57205,10 +57281,10 @@
         <v>1</v>
       </c>
       <c r="D56" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E56" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F56" s="39">
         <v>62</v>
@@ -58232,9 +58308,9 @@
       <c r="AMI56"/>
       <c r="AMJ56"/>
     </row>
-    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1024">
       <c r="A57" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" s="22" t="s">
         <v>12</v>
@@ -58246,13 +58322,13 @@
         <v>10252</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F57" s="2">
         <v>1450</v>
       </c>
       <c r="G57" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H57" s="22">
         <v>250</v>
@@ -59274,9 +59350,9 @@
       <c r="AMI57"/>
       <c r="AMJ57"/>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1024">
       <c r="A58" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B58" s="41" t="s">
         <v>12</v>
@@ -59288,7 +59364,7 @@
         <v>10252</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F58" s="39">
         <v>49.97945</v>
@@ -60312,9 +60388,9 @@
       <c r="AMI58"/>
       <c r="AMJ58"/>
     </row>
-    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1024">
       <c r="A59" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="41" t="s">
         <v>12</v>
@@ -60326,7 +60402,7 @@
         <v>10252</v>
       </c>
       <c r="E59" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F59" s="39">
         <v>-144.254166666667</v>
@@ -61350,9 +61426,9 @@
       <c r="AMI59"/>
       <c r="AMJ59"/>
     </row>
-    <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1024">
       <c r="A60" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>12</v>
@@ -61364,7 +61440,7 @@
         <v>10252</v>
       </c>
       <c r="E60" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F60" s="39">
         <v>52</v>
@@ -62388,9 +62464,9 @@
       <c r="AMI60"/>
       <c r="AMJ60"/>
     </row>
-    <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1024">
       <c r="A61" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>12</v>
@@ -62402,13 +62478,13 @@
         <v>10219</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F61" s="2">
         <v>1450</v>
       </c>
       <c r="G61" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H61" s="22">
         <v>350</v>
@@ -63430,9 +63506,9 @@
       <c r="AMI61"/>
       <c r="AMJ61"/>
     </row>
-    <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1024">
       <c r="A62" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" s="41" t="s">
         <v>12</v>
@@ -63444,7 +63520,7 @@
         <v>10219</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F62" s="39">
         <v>49.97945</v>
@@ -64468,9 +64544,9 @@
       <c r="AMI62"/>
       <c r="AMJ62"/>
     </row>
-    <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1024">
       <c r="A63" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" s="41" t="s">
         <v>12</v>
@@ -64482,7 +64558,7 @@
         <v>10219</v>
       </c>
       <c r="E63" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F63" s="39">
         <v>-144.254166666667</v>
@@ -65506,9 +65582,9 @@
       <c r="AMI63"/>
       <c r="AMJ63"/>
     </row>
-    <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1024">
       <c r="A64" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="41" t="s">
         <v>12</v>
@@ -65520,7 +65596,7 @@
         <v>10219</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F64" s="39">
         <v>19</v>
@@ -66544,9 +66620,9 @@
       <c r="AMI64"/>
       <c r="AMJ64"/>
     </row>
-    <row r="65" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1024">
       <c r="A65" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>12</v>
@@ -66558,13 +66634,13 @@
         <v>10256</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F65" s="2">
         <v>1450</v>
       </c>
       <c r="G65" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H65" s="22">
         <v>501</v>
@@ -67586,9 +67662,9 @@
       <c r="AMI65"/>
       <c r="AMJ65"/>
     </row>
-    <row r="66" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1024">
       <c r="A66" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="41" t="s">
         <v>12</v>
@@ -67600,7 +67676,7 @@
         <v>10256</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F66" s="39">
         <v>49.97945</v>
@@ -68624,9 +68700,9 @@
       <c r="AMI66"/>
       <c r="AMJ66"/>
     </row>
-    <row r="67" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1024">
       <c r="A67" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" s="41" t="s">
         <v>12</v>
@@ -68638,7 +68714,7 @@
         <v>10256</v>
       </c>
       <c r="E67" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F67" s="39">
         <v>-144.254166666667</v>
@@ -69662,9 +69738,9 @@
       <c r="AMI67"/>
       <c r="AMJ67"/>
     </row>
-    <row r="68" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1024">
       <c r="A68" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="41" t="s">
         <v>12</v>
@@ -69676,7 +69752,7 @@
         <v>10256</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F68" s="39">
         <v>56</v>
@@ -70700,9 +70776,9 @@
       <c r="AMI68"/>
       <c r="AMJ68"/>
     </row>
-    <row r="69" spans="1:1024" s="51" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1024" s="51" customFormat="1">
       <c r="A69" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" s="48" t="s">
         <v>12</v>
@@ -70714,22 +70790,22 @@
         <v>10226</v>
       </c>
       <c r="E69" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F69" s="1">
         <v>5076</v>
       </c>
       <c r="G69" s="50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H69" s="48">
         <v>748</v>
       </c>
       <c r="J69" s="48"/>
     </row>
-    <row r="70" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1024">
       <c r="A70" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="52" t="s">
         <v>12</v>
@@ -70741,7 +70817,7 @@
         <v>10226</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F70" s="39">
         <v>49.97945</v>
@@ -70750,9 +70826,9 @@
       <c r="H70"/>
       <c r="J70" s="22"/>
     </row>
-    <row r="71" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1024">
       <c r="A71" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="52" t="s">
         <v>12</v>
@@ -70764,7 +70840,7 @@
         <v>10226</v>
       </c>
       <c r="E71" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F71" s="39">
         <v>-144.254166666667</v>
@@ -70773,9 +70849,9 @@
       <c r="H71"/>
       <c r="J71" s="22"/>
     </row>
-    <row r="72" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1024">
       <c r="A72" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="52" t="s">
         <v>12</v>
@@ -70787,7 +70863,7 @@
         <v>10226</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F72" s="39">
         <v>26</v>
@@ -70796,9 +70872,9 @@
       <c r="H72"/>
       <c r="J72" s="22"/>
     </row>
-    <row r="73" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1024">
       <c r="A73" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>12</v>
@@ -70810,22 +70886,22 @@
         <v>10229</v>
       </c>
       <c r="E73" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F73" s="1">
         <v>5076</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H73" s="22">
         <v>999</v>
       </c>
       <c r="J73" s="22"/>
     </row>
-    <row r="74" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1024">
       <c r="A74" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" s="41" t="s">
         <v>12</v>
@@ -70837,7 +70913,7 @@
         <v>10229</v>
       </c>
       <c r="E74" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F74" s="39">
         <v>49.97945</v>
@@ -70846,9 +70922,9 @@
       <c r="H74"/>
       <c r="J74" s="22"/>
     </row>
-    <row r="75" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1024">
       <c r="A75" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75" s="41" t="s">
         <v>12</v>
@@ -70860,7 +70936,7 @@
         <v>10229</v>
       </c>
       <c r="E75" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F75" s="39">
         <v>-144.254166666667</v>
@@ -70869,9 +70945,9 @@
       <c r="H75"/>
       <c r="J75" s="22"/>
     </row>
-    <row r="76" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1024">
       <c r="A76" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B76" s="41" t="s">
         <v>12</v>
@@ -70883,7 +70959,7 @@
         <v>10229</v>
       </c>
       <c r="E76" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F76" s="39">
         <v>29</v>
@@ -70892,9 +70968,9 @@
       <c r="H76"/>
       <c r="J76" s="22"/>
     </row>
-    <row r="77" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1024">
       <c r="A77" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>12</v>
@@ -70906,22 +70982,22 @@
         <v>10267</v>
       </c>
       <c r="E77" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F77" s="1">
         <v>5076</v>
       </c>
       <c r="G77" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H77" s="22">
         <v>1501</v>
       </c>
       <c r="J77" s="22"/>
     </row>
-    <row r="78" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1024">
       <c r="A78" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B78" s="41" t="s">
         <v>12</v>
@@ -70933,16 +71009,16 @@
         <v>10267</v>
       </c>
       <c r="E78" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F78" s="39">
         <v>49.97945</v>
       </c>
       <c r="J78" s="22"/>
     </row>
-    <row r="79" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1024">
       <c r="A79" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" s="41" t="s">
         <v>12</v>
@@ -70954,16 +71030,16 @@
         <v>10267</v>
       </c>
       <c r="E79" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F79" s="39">
         <v>-144.254166666667</v>
       </c>
       <c r="J79" s="22"/>
     </row>
-    <row r="80" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1024">
       <c r="A80" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" s="41" t="s">
         <v>12</v>
@@ -70975,19 +71051,19 @@
         <v>10267</v>
       </c>
       <c r="E80" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F80" s="39">
         <v>67</v>
       </c>
       <c r="J80" s="22"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="J81" s="22"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="6" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>12</v>
@@ -70996,15 +71072,15 @@
         <v>1</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>12</v>
@@ -71013,14 +71089,19 @@
         <v>1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>